<commit_message>
gradient boosting (nao funciona)
</commit_message>
<xml_diff>
--- a/grupo/grupo resultados.xlsx
+++ b/grupo/grupo resultados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaol\Desktop\Universidade\4º Ano\1º Semestre\DAA\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaol\Desktop\Universidade\4º Ano\1º Semestre\DAA\Projeto\tp-daa\grupo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C34ED5-2EE7-414D-AA37-9DB28583D094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615AA40B-2206-4957-95CC-011ACA8E00C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B68EDA6F-1AA5-4CD8-9A74-843A2F3B6DD8}"/>
   </bookViews>
@@ -190,10 +190,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -563,7 +563,7 @@
   <dimension ref="C2:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:R8"/>
+      <selection activeCell="Q10" sqref="Q10:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,37 +572,37 @@
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="5"/>
       <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="6"/>
+      <c r="N2" s="5"/>
       <c r="O2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="6"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="6"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="6"/>
+      <c r="T2" s="5"/>
       <c r="U2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="6"/>
+      <c r="V2" s="5"/>
     </row>
     <row r="3" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
@@ -1240,72 +1240,84 @@
     </row>
   </sheetData>
   <mergeCells count="168">
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="C19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
     <mergeCell ref="C15:J15"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="M16:N16"/>
@@ -1330,90 +1342,78 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="U14:V14"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="C19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
   </mergeCells>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="top10" dxfId="6" priority="40" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M1">
-    <cfRule type="top10" dxfId="6" priority="6" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="5" priority="40" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="6" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
     <cfRule type="top10" dxfId="4" priority="43" bottom="1" rank="1"/>

</xml_diff>

<commit_message>
eliminacao de coisas inuteis
</commit_message>
<xml_diff>
--- a/grupo/grupo resultados.xlsx
+++ b/grupo/grupo resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaol\Desktop\Universidade\4º Ano\1º Semestre\DAA\Projeto\tp-daa\grupo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF220550-B982-4E6D-ABE4-7402438C3B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9D04F3-4CFC-41E2-BE25-97F6094A1D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B68EDA6F-1AA5-4CD8-9A74-843A2F3B6DD8}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B68EDA6F-1AA5-4CD8-9A74-843A2F3B6DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="23">
   <si>
     <t>MAE</t>
   </si>
@@ -56,100 +56,55 @@
     <t>avg. RMSE</t>
   </si>
   <si>
-    <t>RL (sem index,throws,sh,teamID)</t>
-  </si>
-  <si>
-    <t>RFR (sem index,throws,sh,teamID)</t>
-  </si>
-  <si>
-    <t>DTR (sem index,throws,sh,teamID)</t>
-  </si>
-  <si>
-    <t>NN[3 layers, 32-16-1] (sem index,throws,sh,teamID)</t>
-  </si>
-  <si>
-    <t>SVR[2 folds, 8 candidates, 16 fits] (sem index,throws,sh,teamID)</t>
-  </si>
-  <si>
     <t>Modelos</t>
   </si>
   <si>
-    <t>RL (todas variaveis com inteiros) (ln2)</t>
-  </si>
-  <si>
-    <t>RL (sem index e throws) (ln3)</t>
-  </si>
-  <si>
-    <t>RL (sem label encoding) (ln1)</t>
-  </si>
-  <si>
-    <t>SVR[2 folds, 8 candidates, 16 fits] (todos os inteiros) (svr2)</t>
-  </si>
-  <si>
-    <t>SVR[2 folds, 8 candidates, 16 fits] (sem index e throws) (svr3)</t>
-  </si>
-  <si>
-    <t>SVR[2 folds, 8 candidates, 16 fits] (sem label encoding) (svr1)</t>
-  </si>
-  <si>
-    <t>DTR (todos os inteiros) (2)</t>
-  </si>
-  <si>
-    <t>DTR (sem index e throws) (3)</t>
-  </si>
-  <si>
-    <t>DTR (sem label encoding) (1)</t>
-  </si>
-  <si>
-    <t>RFR (sem label encoding) (1)</t>
-  </si>
-  <si>
-    <t>RFR (todos os inteiros) (2)</t>
-  </si>
-  <si>
-    <t>RFR (sem index e throws) (3)</t>
-  </si>
-  <si>
-    <t>LR (sem index e throws) (3)</t>
-  </si>
-  <si>
-    <t>LR (todos os inteiros) (2)</t>
-  </si>
-  <si>
-    <t>LR (sem label encoding) (1)</t>
-  </si>
-  <si>
-    <t>NN[3 layers, 32-16-1, 5 epochs, batch 10]  (sem index e throws) (3)</t>
-  </si>
-  <si>
-    <t>NN[3 layers, 32-16-1, 5 epochs, batch 10] (todos os inteiros) (2)</t>
-  </si>
-  <si>
     <t>3445777.8</t>
-  </si>
-  <si>
-    <t>GB (sem label encoding) (1)</t>
-  </si>
-  <si>
-    <t>GB (todos os inteiros) (2)</t>
-  </si>
-  <si>
-    <t>GB (sem index e throws) (3)</t>
-  </si>
-  <si>
-    <t>XGB (sem label encoding) (1)</t>
-  </si>
-  <si>
-    <t>XGB (todos os inteiros) (2)</t>
-  </si>
-  <si>
-    <t>XGB (sem index e throws) (3)</t>
   </si>
   <si>
     <t>184617,.0</t>
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Versão</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>DTR</t>
+  </si>
+  <si>
+    <t>RFR</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>XGB</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>NN [3 layers, 32-16-1, 5 epochs, batch 10]</t>
+  </si>
+  <si>
+    <t>SVR [2 folds, 8 candidates, 16 fits]</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>VExtra</t>
   </si>
 </sst>
 </file>
@@ -229,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -274,11 +229,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,86 +293,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,61 +1093,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D30CEC0-1B37-4F2D-B97E-4A8938D00681}">
-  <dimension ref="C2:V30"/>
+  <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30:R30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="28"/>
+      <c r="M2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="28"/>
+      <c r="O2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="28"/>
+      <c r="S2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="28"/>
+      <c r="U2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="28"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="T2" s="5"/>
-      <c r="U2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V2" s="5"/>
-    </row>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
+      <c r="C3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="1">
         <v>1921803.3280790001</v>
       </c>
@@ -1147,17 +1179,18 @@
       </c>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1">
         <v>1920016.15150204</v>
       </c>
@@ -1183,17 +1216,18 @@
       </c>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
+      <c r="C5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
       <c r="K5" s="1">
         <v>1921540.52098138</v>
       </c>
@@ -1219,17 +1253,18 @@
       </c>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="33"/>
+      <c r="C6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="1">
         <v>1922266.8425652699</v>
       </c>
@@ -1255,17 +1290,20 @@
       </c>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="1">
         <v>1996612.99269557</v>
       </c>
@@ -1279,29 +1317,30 @@
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C8" s="15" t="s">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
+      <c r="C8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="1">
         <v>1996660.9650094199</v>
       </c>
@@ -1315,29 +1354,30 @@
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="1">
         <v>2068477.5315739801</v>
       </c>
@@ -1351,29 +1391,30 @@
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="1">
         <v>2118442.4836239298</v>
       </c>
@@ -1387,29 +1428,32 @@
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="1">
         <v>1573553.4935850599</v>
       </c>
@@ -1423,29 +1467,30 @@
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C12" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="1">
         <v>1550662.94835061</v>
       </c>
@@ -1459,29 +1504,30 @@
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C13" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="1">
         <v>1603397.8937478501</v>
       </c>
@@ -1495,29 +1541,30 @@
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T13" s="2"/>
       <c r="U13" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="33"/>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="1">
         <v>1637409.71017306</v>
       </c>
@@ -1531,29 +1578,32 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T14" s="2"/>
       <c r="U14" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="1">
         <v>2285162</v>
       </c>
@@ -1563,33 +1613,34 @@
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="1">
         <v>2229383</v>
       </c>
@@ -1603,29 +1654,30 @@
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T16" s="2"/>
       <c r="U16" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="36"/>
+      <c r="C17" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="1">
         <v>2068477.5315739801</v>
       </c>
@@ -1639,29 +1691,32 @@
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T17" s="2"/>
       <c r="U17" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C18" s="12" t="s">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="1">
         <v>1708596.24495021</v>
       </c>
@@ -1675,29 +1730,30 @@
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T18" s="2"/>
       <c r="U18" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="35"/>
+      <c r="C19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="1">
         <v>1708207.04132546</v>
       </c>
@@ -1711,29 +1767,30 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T19" s="2"/>
       <c r="U19" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="35"/>
+      <c r="C20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="1">
         <v>1708206.31558144</v>
       </c>
@@ -1747,29 +1804,30 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T20" s="2"/>
       <c r="U20" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C21" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="36"/>
+      <c r="C21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="17"/>
       <c r="K21" s="1">
         <v>1708197.8560689699</v>
       </c>
@@ -1783,29 +1841,32 @@
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T21" s="2"/>
       <c r="U21" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C22" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
       <c r="K22" s="1">
         <v>1921803.3053353401</v>
       </c>
@@ -1819,29 +1880,30 @@
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T22" s="2"/>
       <c r="U22" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C23" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
+      <c r="C23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="1">
         <v>1920016.1219757199</v>
       </c>
@@ -1855,29 +1917,30 @@
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T23" s="2"/>
       <c r="U23" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C24" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="33"/>
+      <c r="C24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
       <c r="K24" s="1">
         <v>1921540.4968103899</v>
       </c>
@@ -1891,29 +1954,32 @@
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T24" s="2"/>
       <c r="U24" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C25" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="1">
         <v>1855702.0007390201</v>
       </c>
@@ -1927,29 +1993,30 @@
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T25" s="2"/>
       <c r="U25" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C26" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
+      <c r="C26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
       <c r="K26" s="1">
         <v>1857735.2350820401</v>
       </c>
@@ -1963,29 +2030,30 @@
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C27" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26"/>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="33"/>
+      <c r="C27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="1">
         <v>1863113.53523336</v>
       </c>
@@ -1999,31 +2067,34 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T27" s="2"/>
       <c r="U27" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C28" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="29"/>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="1">
@@ -2035,29 +2106,30 @@
       </c>
       <c r="P28" s="2"/>
       <c r="Q28" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C29" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="29"/>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="32"/>
+      <c r="C29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
       <c r="K29" s="1">
         <v>1842290</v>
       </c>
@@ -2071,29 +2143,30 @@
       </c>
       <c r="P29" s="2"/>
       <c r="Q29" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C30" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="29"/>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="33"/>
+      <c r="C30" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
       <c r="K30" s="1">
         <v>1843538.1</v>
       </c>
@@ -2107,48 +2180,172 @@
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="T30" s="2"/>
       <c r="U30" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="V30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="203">
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="U26:V26"/>
+  <mergeCells count="211">
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="C19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
@@ -2173,136 +2370,17 @@
     <mergeCell ref="C29:J29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="C19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:V26"/>
     <mergeCell ref="U24:V24"/>
     <mergeCell ref="S24:T24"/>
     <mergeCell ref="Q24:R24"/>
@@ -2310,20 +2388,23 @@
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="C24:J24"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
   </mergeCells>
   <conditionalFormatting sqref="K34:K1048576 K1:K30">
     <cfRule type="top10" dxfId="54" priority="200" bottom="1" rank="1"/>
@@ -2340,155 +2421,155 @@
   <conditionalFormatting sqref="Q34:Q1048576 Q1:Q30">
     <cfRule type="top10" dxfId="50" priority="209" bottom="1" rank="1"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S7">
+    <cfRule type="top10" dxfId="49" priority="48" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S8">
+    <cfRule type="top10" dxfId="48" priority="45" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S9">
+    <cfRule type="top10" dxfId="47" priority="44" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10">
+    <cfRule type="top10" dxfId="46" priority="42" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S11">
+    <cfRule type="top10" dxfId="45" priority="40" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S12">
+    <cfRule type="top10" dxfId="44" priority="38" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13">
+    <cfRule type="top10" dxfId="43" priority="36" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S14">
+    <cfRule type="top10" dxfId="42" priority="34" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S15">
+    <cfRule type="top10" dxfId="41" priority="32" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S16">
+    <cfRule type="top10" dxfId="40" priority="30" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S17">
+    <cfRule type="top10" dxfId="39" priority="28" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S18">
+    <cfRule type="top10" dxfId="38" priority="26" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S19">
+    <cfRule type="top10" dxfId="37" priority="24" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20">
+    <cfRule type="top10" dxfId="36" priority="22" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S21">
+    <cfRule type="top10" dxfId="35" priority="20" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S22">
+    <cfRule type="top10" dxfId="34" priority="18" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S23">
+    <cfRule type="top10" dxfId="33" priority="16" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S24">
+    <cfRule type="top10" dxfId="32" priority="14" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S25">
+    <cfRule type="top10" dxfId="31" priority="12" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S26">
+    <cfRule type="top10" dxfId="30" priority="10" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S27">
+    <cfRule type="top10" dxfId="29" priority="8" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S28">
+    <cfRule type="top10" dxfId="28" priority="6" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S29">
+    <cfRule type="top10" dxfId="27" priority="4" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S30">
+    <cfRule type="top10" dxfId="26" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S34:S1048576 S1:S6">
-    <cfRule type="top10" dxfId="49" priority="212" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U34:U1048576 U1:U6">
-    <cfRule type="top10" dxfId="48" priority="215" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S7">
-    <cfRule type="top10" dxfId="47" priority="48" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="212" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7">
-    <cfRule type="top10" dxfId="46" priority="47" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="47" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8">
-    <cfRule type="top10" dxfId="45" priority="46" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S8">
-    <cfRule type="top10" dxfId="44" priority="45" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
-    <cfRule type="top10" dxfId="43" priority="44" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="46" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U9">
-    <cfRule type="top10" dxfId="42" priority="43" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
-    <cfRule type="top10" dxfId="41" priority="42" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="43" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U10">
-    <cfRule type="top10" dxfId="40" priority="41" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="top10" dxfId="39" priority="40" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="41" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11">
-    <cfRule type="top10" dxfId="38" priority="39" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="top10" dxfId="37" priority="38" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="39" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12">
-    <cfRule type="top10" dxfId="36" priority="37" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
-    <cfRule type="top10" dxfId="35" priority="36" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="37" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13">
-    <cfRule type="top10" dxfId="34" priority="35" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="top10" dxfId="33" priority="34" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="35" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14">
-    <cfRule type="top10" dxfId="32" priority="33" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S15">
-    <cfRule type="top10" dxfId="31" priority="32" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="33" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15">
-    <cfRule type="top10" dxfId="30" priority="31" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S16">
-    <cfRule type="top10" dxfId="29" priority="30" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="31" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16">
-    <cfRule type="top10" dxfId="28" priority="29" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
-    <cfRule type="top10" dxfId="27" priority="28" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="29" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U17">
-    <cfRule type="top10" dxfId="26" priority="27" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
-    <cfRule type="top10" dxfId="25" priority="26" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="27" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U18">
-    <cfRule type="top10" dxfId="24" priority="25" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S19">
-    <cfRule type="top10" dxfId="23" priority="24" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="25" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U19">
-    <cfRule type="top10" dxfId="22" priority="23" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S20">
-    <cfRule type="top10" dxfId="21" priority="22" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="23" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U20">
-    <cfRule type="top10" dxfId="20" priority="21" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S21">
-    <cfRule type="top10" dxfId="19" priority="20" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="21" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U21">
-    <cfRule type="top10" dxfId="18" priority="19" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S22">
-    <cfRule type="top10" dxfId="17" priority="18" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="19" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="top10" dxfId="16" priority="17" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S23">
-    <cfRule type="top10" dxfId="15" priority="16" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="17" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U23">
-    <cfRule type="top10" dxfId="14" priority="15" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S24">
-    <cfRule type="top10" dxfId="13" priority="14" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="15" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U24">
-    <cfRule type="top10" dxfId="12" priority="13" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S25">
-    <cfRule type="top10" dxfId="11" priority="12" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="13" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U25">
-    <cfRule type="top10" dxfId="10" priority="11" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
-    <cfRule type="top10" dxfId="9" priority="10" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="11" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U26">
-    <cfRule type="top10" dxfId="8" priority="9" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S27">
-    <cfRule type="top10" dxfId="7" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="9" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U27">
-    <cfRule type="top10" dxfId="6" priority="7" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S28">
-    <cfRule type="top10" dxfId="5" priority="6" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="7" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28">
-    <cfRule type="top10" dxfId="4" priority="5" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S29">
-    <cfRule type="top10" dxfId="3" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="5" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U29">
     <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S30">
-    <cfRule type="top10" dxfId="1" priority="2" bottom="1" rank="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="U30">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U34:U1048576 U1:U6">
+    <cfRule type="top10" dxfId="0" priority="215" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>